<commit_message>
🔼 Atualização no banco de dados
Adição da linha "jogos" do tipo array na coleção usuários
</commit_message>
<xml_diff>
--- a/BD/DicionárioDeDados_Nanni_Community.xlsx
+++ b/BD/DicionárioDeDados_Nanni_Community.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
   <si>
     <t>Coleção Usuários</t>
   </si>
@@ -50,6 +50,27 @@
   </si>
   <si>
     <t>data de nascimento especificada pelo usuário</t>
+  </si>
+  <si>
+    <t>nomeUser</t>
+  </si>
+  <si>
+    <t>nome/apelido do usuário</t>
+  </si>
+  <si>
+    <t>numFollow</t>
+  </si>
+  <si>
+    <t>numero de seguidores do usuário</t>
+  </si>
+  <si>
+    <t>jogos</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>array com referencias aos jogos do usuario</t>
   </si>
   <si>
     <t>avatarUser</t>
@@ -239,9 +260,6 @@
   </si>
   <si>
     <t>anexoDisc</t>
-  </si>
-  <si>
-    <t>array</t>
   </si>
   <si>
     <t>array que carrega os anexos(imagem/gif) da mensagem da discussão</t>
@@ -813,474 +831,507 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="12" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C13" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="8" t="s">
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="C14" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="C16" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="18" t="s">
+      <c r="C17" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B20" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C20" s="20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="22" t="s">
+    <row r="21">
+      <c r="A21" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>36</v>
+      <c r="C21" s="23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="s">
+      <c r="C26" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="25" t="s">
+    <row r="30">
+      <c r="A30" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="C30" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>50</v>
+      <c r="C31" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
+      <c r="A32" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B36" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C36" s="16" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="14" t="s">
+      <c r="C43" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B46" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C46" s="16" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="3"/>
+      <c r="C50" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B54" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B55" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B56" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" s="12" t="s">
+      <c r="A56" s="7" t="s">
         <v>85</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>